<commit_message>
"Added changes to home page and style.css files. Added cool buttons!"
</commit_message>
<xml_diff>
--- a/appointments.xlsx
+++ b/appointments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Deep Chakravorty</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9875480108</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>I don't know.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-21 13:35:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
"Added few videos and photos for gallery and also better style.css"
</commit_message>
<xml_diff>
--- a/appointments.xlsx
+++ b/appointments.xlsx
@@ -1,34 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\Clinic web\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Divit Chakravorty</t>
+  </si>
+  <si>
+    <t>9880188877</t>
+  </si>
+  <si>
+    <t>wdgergdgdgdrgdg or Something related to phobias</t>
+  </si>
+  <si>
+    <t>Deep Chakravorty</t>
+  </si>
+  <si>
+    <t>9875480108</t>
+  </si>
+  <si>
+    <t>I don't know.</t>
+  </si>
+  <si>
+    <t>2025-09-21 13:35:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>2e</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +94,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,73 +396,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Full Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Reason</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Divit Chakravorty</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9880188877</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>wdgergdgdgdrgdg or Something related to phobias</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Deep Chakravorty</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>9875480108</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>I don't know.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-09-21 13:35:00</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Tried to fix Python backend. Created awareness page and linked it to homepage. Edited meet the doctor page to fix scroll to top button. Edited whatsapp link on homepage."
</commit_message>
<xml_diff>
--- a/appointments.xlsx
+++ b/appointments.xlsx
@@ -1,81 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\Clinic web\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Reason</t>
-  </si>
-  <si>
-    <t>Divit Chakravorty</t>
-  </si>
-  <si>
-    <t>9880188877</t>
-  </si>
-  <si>
-    <t>wdgergdgdgdrgdg or Something related to phobias</t>
-  </si>
-  <si>
-    <t>Deep Chakravorty</t>
-  </si>
-  <si>
-    <t>9875480108</t>
-  </si>
-  <si>
-    <t>I don't know.</t>
-  </si>
-  <si>
-    <t>2025-09-21 13:35:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>2e</t>
-  </si>
-  <si>
-    <t>e2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,132 +407,300 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Divit Chakravorty</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>wdgergdgdgdrgdg or Something related to phobias</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Deep Chakravorty</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>9875480108</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>I don't know.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-21 13:35:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Idk for realkjsdn lkajshg erdfjh .</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:30:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Idk realistically just for testing</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:47:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>For testing</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:50:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>For Testing</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:52:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>s5rtdytjtyjytj</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:54:17</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Mission accomplished!! Ready for the web!!"
</commit_message>
<xml_diff>
--- a/appointments.xlsx
+++ b/appointments.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -703,6 +703,28 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Nishant</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>9880188877</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Idk</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-10-01 18:06:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>